<commit_message>
proteingroups.txt and results updated
</commit_message>
<xml_diff>
--- a/Example/Limma_output/Final_tsvs/Links.xlsx
+++ b/Example/Limma_output/Final_tsvs/Links.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -377,151 +377,721 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Pet309</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mrp49</t>
+          <t>Mgr1</t>
         </is>
       </c>
       <c r="C2">
-        <v>1.52827182145422</v>
+        <v>2.73192036248588</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Pet309</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Aep1</t>
+          <t>Yfr045w</t>
         </is>
       </c>
       <c r="C3">
-        <v>1.503685756493</v>
+        <v>4.29155076094434</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Pet309</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ylf2</t>
+          <t>Pgk1</t>
         </is>
       </c>
       <c r="C4">
-        <v>2.06717112217523</v>
+        <v>2.6873712653173</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Pet309</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Rpm2</t>
+          <t>Cyt1</t>
         </is>
       </c>
       <c r="C5">
-        <v>2.46905970871401</v>
+        <v>4.50985096362768</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Cbp1</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Atp25</t>
+          <t>Cbp6</t>
         </is>
       </c>
       <c r="C6">
-        <v>1.80941184846945</v>
+        <v>4.35868327812307</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cbp1</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Mgr1</t>
+          <t>Lpd1</t>
         </is>
       </c>
       <c r="C7">
-        <v>1.79649508184685</v>
+        <v>1.57503563543666</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Cbp1</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mrp49</t>
+          <t>Sal1</t>
         </is>
       </c>
       <c r="C8">
-        <v>1.69388126648138</v>
+        <v>2.02978454788679</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Cbp1</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ylf2</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="C9">
-        <v>2.69358745023701</v>
+        <v>8.224277944134281</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Cbp1</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Mss2</t>
+          <t>Yme1</t>
         </is>
       </c>
       <c r="C10">
-        <v>1.92708120439405</v>
+        <v>2.46946334757457</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Cbp1</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>Nat2</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>3.64365949026057</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Mba1</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>1.83831970980128</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Ylf2</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>2.11826752070948</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Cox15</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>2.27996690169153</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Mmf1</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>1.78419300713538</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Nde1</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>3.06117027536866</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Coa1</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>5.69366488074423</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>Tes1</t>
         </is>
       </c>
-      <c r="C11">
-        <v>3.14621322828423</v>
+      <c r="C18">
+        <v>2.9134727941155</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Ydl183c</t>
+        </is>
+      </c>
+      <c r="C19">
+        <v>2.33166543247548</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Ynr040w</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>1.62948982493171</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Tim11</t>
+        </is>
+      </c>
+      <c r="C21">
+        <v>1.70713143459762</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Tim50</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>3.93811928468223</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Ydl027c</t>
+        </is>
+      </c>
+      <c r="C23">
+        <v>2.98248517028716</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Fmp25</t>
+        </is>
+      </c>
+      <c r="C24">
+        <v>3.945283109823</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Mdm38</t>
+        </is>
+      </c>
+      <c r="C25">
+        <v>1.83748868148113</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Rdl2</t>
+        </is>
+      </c>
+      <c r="C26">
+        <v>1.79841819588168</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Ypl168w</t>
+        </is>
+      </c>
+      <c r="C27">
+        <v>5.99745123535862</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Mgr1</t>
+        </is>
+      </c>
+      <c r="C28">
+        <v>2.66641681329914</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Yfr045w</t>
+        </is>
+      </c>
+      <c r="C29">
+        <v>4.4764061505584</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Cyt1</t>
+        </is>
+      </c>
+      <c r="C30">
+        <v>2.62702982182357</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Cbp6</t>
+        </is>
+      </c>
+      <c r="C31">
+        <v>6.07391985618894</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Sal1</t>
+        </is>
+      </c>
+      <c r="C32">
+        <v>2.45266055651041</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="C33">
+        <v>4.52570231746408</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Mrp20</t>
+        </is>
+      </c>
+      <c r="C34">
+        <v>4.15303630443696</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Nat2</t>
+        </is>
+      </c>
+      <c r="C35">
+        <v>3.23015931185425</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Mcx1</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>2.43331292363129</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Ylf2</t>
+        </is>
+      </c>
+      <c r="C37">
+        <v>2.66622117737042</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Cox15</t>
+        </is>
+      </c>
+      <c r="C38">
+        <v>2.37818415438592</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Mmf1</t>
+        </is>
+      </c>
+      <c r="C39">
+        <v>1.74962157922412</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Nde1</t>
+        </is>
+      </c>
+      <c r="C40">
+        <v>2.1543647792905</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Coa1</t>
+        </is>
+      </c>
+      <c r="C41">
+        <v>4.27816698884227</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Tes1</t>
+        </is>
+      </c>
+      <c r="C42">
+        <v>3.10335481478691</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Ydl183c</t>
+        </is>
+      </c>
+      <c r="C43">
+        <v>2.13977246877701</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Ynr040w</t>
+        </is>
+      </c>
+      <c r="C44">
+        <v>2.64464089095586</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Tim11</t>
+        </is>
+      </c>
+      <c r="C45">
+        <v>1.76656486889668</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Tim50</t>
+        </is>
+      </c>
+      <c r="C46">
+        <v>3.09184685452373</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Ydl027c</t>
+        </is>
+      </c>
+      <c r="C47">
+        <v>2.62080027942017</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Rdl2</t>
+        </is>
+      </c>
+      <c r="C48">
+        <v>2.42682535503346</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Mrpl4</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Ypl168w</t>
+        </is>
+      </c>
+      <c r="C49">
+        <v>6.69131505804129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added filter based on sequence coverage and unique peptides
</commit_message>
<xml_diff>
--- a/Example/Limma_output/Final_tsvs/Links.xlsx
+++ b/Example/Limma_output/Final_tsvs/Links.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -377,7 +377,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -386,13 +386,13 @@
         </is>
       </c>
       <c r="C2">
-        <v>2.73192036248588</v>
+        <v>2.242187785</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -401,307 +401,307 @@
         </is>
       </c>
       <c r="C3">
-        <v>4.29155076094434</v>
+        <v>4.476406151</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Pgk1</t>
+          <t>Cyt1</t>
         </is>
       </c>
       <c r="C4">
-        <v>2.6873712653173</v>
+        <v>2.627029822</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cyt1</t>
+          <t>Cbp6</t>
         </is>
       </c>
       <c r="C5">
-        <v>4.50985096362768</v>
+        <v>6.073919856</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cbp6</t>
+          <t>Pet111</t>
         </is>
       </c>
       <c r="C6">
-        <v>4.35868327812307</v>
+        <v>1.779152136</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lpd1</t>
+          <t>Sal1</t>
         </is>
       </c>
       <c r="C7">
-        <v>1.57503563543666</v>
+        <v>2.500020235</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sal1</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="C8">
-        <v>2.02978454788679</v>
+        <v>4.525702317</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrp20</t>
         </is>
       </c>
       <c r="C9">
-        <v>8.224277944134281</v>
+        <v>4.153036304</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Yme1</t>
+          <t>Nat2</t>
         </is>
       </c>
       <c r="C10">
-        <v>2.46946334757457</v>
+        <v>4.078817589</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Nat2</t>
+          <t>Mba1</t>
         </is>
       </c>
       <c r="C11">
-        <v>3.64365949026057</v>
+        <v>2.061652968</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Mba1</t>
+          <t>Mcx1</t>
         </is>
       </c>
       <c r="C12">
-        <v>1.83831970980128</v>
+        <v>1.686755299</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ylf2</t>
+          <t>Cox15</t>
         </is>
       </c>
       <c r="C13">
-        <v>2.11826752070948</v>
+        <v>2.378184154</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Cox15</t>
+          <t>Mmf1</t>
         </is>
       </c>
       <c r="C14">
-        <v>2.27996690169153</v>
+        <v>1.749621579</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Mmf1</t>
+          <t>Nde1</t>
         </is>
       </c>
       <c r="C15">
-        <v>1.78419300713538</v>
+        <v>2.154364779</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Nde1</t>
+          <t>Coa1</t>
         </is>
       </c>
       <c r="C16">
-        <v>3.06117027536866</v>
+        <v>5.304607176</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Coa1</t>
+          <t>Tes1</t>
         </is>
       </c>
       <c r="C17">
-        <v>5.69366488074423</v>
+        <v>3.103354815</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Tes1</t>
+          <t>Ydl183c</t>
         </is>
       </c>
       <c r="C18">
-        <v>2.9134727941155</v>
+        <v>2.139772469</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Ydl183c</t>
+          <t>Ynr040w</t>
         </is>
       </c>
       <c r="C19">
-        <v>2.33166543247548</v>
+        <v>2.644640891</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ynr040w</t>
+          <t>Tim50</t>
         </is>
       </c>
       <c r="C20">
-        <v>1.62948982493171</v>
+        <v>3.091846855</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Tim11</t>
+          <t>Ydl027c</t>
         </is>
       </c>
       <c r="C21">
-        <v>1.70713143459762</v>
+        <v>2.620800279</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Tim50</t>
+          <t>Rdl2</t>
         </is>
       </c>
       <c r="C22">
-        <v>3.93811928468223</v>
+        <v>2.426825355</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Mrpl4</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Ydl027c</t>
+          <t>Ypl168w</t>
         </is>
       </c>
       <c r="C23">
-        <v>2.98248517028716</v>
+        <v>6.315955929</v>
       </c>
     </row>
     <row r="24">
@@ -712,11 +712,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Fmp25</t>
+          <t>Mgr1</t>
         </is>
       </c>
       <c r="C24">
-        <v>3.945283109823</v>
+        <v>3.037622469</v>
       </c>
     </row>
     <row r="25">
@@ -727,11 +727,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Mdm38</t>
+          <t>Yfr045w</t>
         </is>
       </c>
       <c r="C25">
-        <v>1.83748868148113</v>
+        <v>4.291550761</v>
       </c>
     </row>
     <row r="26">
@@ -742,11 +742,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Rdl2</t>
+          <t>Aim39</t>
         </is>
       </c>
       <c r="C26">
-        <v>1.79841819588168</v>
+        <v>2.005386778</v>
       </c>
     </row>
     <row r="27">
@@ -757,137 +757,137 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Ypl168w</t>
+          <t>Pgk1</t>
         </is>
       </c>
       <c r="C27">
-        <v>5.99745123535862</v>
+        <v>2.687371265</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Mgr1</t>
+          <t>Cyt1</t>
         </is>
       </c>
       <c r="C28">
-        <v>2.66641681329914</v>
+        <v>4.509850964</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Yfr045w</t>
+          <t>Cbp6</t>
         </is>
       </c>
       <c r="C29">
-        <v>4.4764061505584</v>
+        <v>4.358683278</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Cyt1</t>
+          <t>Lpd1</t>
         </is>
       </c>
       <c r="C30">
-        <v>2.62702982182357</v>
+        <v>1.575035635</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Cbp6</t>
+          <t>Sal1</t>
         </is>
       </c>
       <c r="C31">
-        <v>6.07391985618894</v>
+        <v>2.591443261</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Sal1</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="C32">
-        <v>2.45266055651041</v>
+        <v>8.224277944000001</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Cbp3</t>
+          <t>Yme1</t>
         </is>
       </c>
       <c r="C33">
-        <v>4.52570231746408</v>
+        <v>2.400876254</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Mrp20</t>
+          <t>Nat2</t>
         </is>
       </c>
       <c r="C34">
-        <v>4.15303630443696</v>
+        <v>3.526374914</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Nat2</t>
+          <t>Mba1</t>
         </is>
       </c>
       <c r="C35">
-        <v>3.23015931185425</v>
+        <v>1.888152295</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -896,13 +896,13 @@
         </is>
       </c>
       <c r="C36">
-        <v>2.43331292363129</v>
+        <v>1.813332533</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -911,13 +911,13 @@
         </is>
       </c>
       <c r="C37">
-        <v>2.66622117737042</v>
+        <v>2.999642688</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -926,13 +926,13 @@
         </is>
       </c>
       <c r="C38">
-        <v>2.37818415438592</v>
+        <v>2.279966902</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -941,13 +941,13 @@
         </is>
       </c>
       <c r="C39">
-        <v>1.74962157922412</v>
+        <v>1.784193007</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -956,13 +956,13 @@
         </is>
       </c>
       <c r="C40">
-        <v>2.1543647792905</v>
+        <v>3.061170275</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -971,13 +971,13 @@
         </is>
       </c>
       <c r="C41">
-        <v>4.27816698884227</v>
+        <v>5.19063741</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -986,13 +986,13 @@
         </is>
       </c>
       <c r="C42">
-        <v>3.10335481478691</v>
+        <v>2.913472794</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1001,13 +1001,13 @@
         </is>
       </c>
       <c r="C43">
-        <v>2.13977246877701</v>
+        <v>2.331665432</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1016,82 +1016,97 @@
         </is>
       </c>
       <c r="C44">
-        <v>2.64464089095586</v>
+        <v>1.629489825</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Tim11</t>
+          <t>Tim50</t>
         </is>
       </c>
       <c r="C45">
-        <v>1.76656486889668</v>
+        <v>3.938119285</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Tim50</t>
+          <t>Ydl027c</t>
         </is>
       </c>
       <c r="C46">
-        <v>3.09184685452373</v>
+        <v>2.98248517</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Ydl027c</t>
+          <t>Fmp25</t>
         </is>
       </c>
       <c r="C47">
-        <v>2.62080027942017</v>
+        <v>3.94528311</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Rdl2</t>
+          <t>Mdm38</t>
         </is>
       </c>
       <c r="C48">
-        <v>2.42682535503346</v>
+        <v>1.837488681</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Mrpl4</t>
+          <t>Cbp3</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
+          <t>Rdl2</t>
+        </is>
+      </c>
+      <c r="C49">
+        <v>1.798418196</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Cbp3</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
           <t>Ypl168w</t>
         </is>
       </c>
-      <c r="C49">
-        <v>6.69131505804129</v>
+      <c r="C50">
+        <v>5.757088287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>